<commit_message>
rm sib sp 61e7e1e7c8d7fe61047dff7e851ec7279dd5483c
</commit_message>
<xml_diff>
--- a/ig/ft/#3-add-narative/StructureDefinition-cds-bundle-transaction-creation.xlsx
+++ b/ig/ft/#3-add-narative/StructureDefinition-cds-bundle-transaction-creation.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-16T11:00:57+00:00</t>
+    <t>2024-02-16T16:08:15+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -954,7 +954,7 @@
   </si>
   <si>
     <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-req-met:POST s'il s’agit d’un nouvel élément ou PUT s'il s’agit d’un élément qui existe déjà {value='POST' or value='PUT'}</t>
+req-met:null {value='POST' or value='PUT'}</t>
   </si>
   <si>
     <t>Bundle.entry:careTeam.request.url</t>

</xml_diff>